<commit_message>
updated historical_weekly.R to  calculate pir for each year then average
</commit_message>
<xml_diff>
--- a/Historical averages through 2021.xlsx
+++ b/Historical averages through 2021.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10714"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/user/Programming Directory/Ebel Lab/wnv-ss-wkly_report/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4ABA016-EB02-9942-8331-4534F6B7435D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F47892F8-A6D1-5745-88B8-077B25CC6CB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-37120" yWindow="80" windowWidth="28800" windowHeight="16220" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Abundance" sheetId="1" r:id="rId1"/>
@@ -792,7 +792,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:AA106"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A9" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="AA4" sqref="AA4"/>
     </sheetView>
   </sheetViews>
@@ -6383,7 +6383,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B2:AA87"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A6" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="Z5" sqref="Z5"/>
     </sheetView>
   </sheetViews>
@@ -11669,8 +11669,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B2:AA89"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AA12" sqref="AA12"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Y2" sqref="Y2:Y20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>